<commit_message>
adesso legeg anche gli adjustment
</commit_message>
<xml_diff>
--- a/template/template.xlsx
+++ b/template/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>4.2.2 Planned outages in the transmission grid and on interconnections</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>last update</t>
-  </si>
-  <si>
-    <t>06 10 2017</t>
   </si>
   <si>
     <t>assets concerned</t>
@@ -65,9 +62,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-410]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="165" formatCode="d/m/yy\ h\.mm;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -146,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -171,26 +167,10 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -549,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +547,7 @@
     <col min="8" max="8" width="4" customWidth="1"/>
     <col min="9" max="9" width="73" customWidth="1"/>
     <col min="10" max="10" width="42.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -594,9 +574,7 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="D3" s="7"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -608,332 +586,44 @@
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="D5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="H5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="18" t="s">
+      <c r="J5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="14"/>
-      <c r="H6" s="15"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="14"/>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="14"/>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="14"/>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="14"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="14"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="14"/>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="14"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="14"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="14"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="14"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="14"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="14"/>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="14"/>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="14"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="14"/>
-      <c r="H21" s="15"/>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="14"/>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="14"/>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="14"/>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="14"/>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="19"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="19"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="19"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="19"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="19"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>